<commit_message>
Add support for actor checking.
</commit_message>
<xml_diff>
--- a/examples/main-voice.xlsx
+++ b/examples/main-voice.xlsx
@@ -25,6 +25,9 @@
     <x:t>Qualifier</x:t>
   </x:si>
   <x:si>
+    <x:t>Actor</x:t>
+  </x:si>
+  <x:si>
     <x:t>Line</x:t>
   </x:si>
   <x:si>
@@ -40,7 +43,7 @@
     <x:t>main_TestScene_16U4</x:t>
   </x:si>
   <x:si>
-    <x:t>ACTOR</x:t>
+    <x:t>LAURA</x:t>
   </x:si>
   <x:si>
     <x:t/>
@@ -65,6 +68,9 @@
   </x:si>
   <x:si>
     <x:t>FRED</x:t>
+  </x:si>
+  <x:si>
+    <x:t>David</x:t>
   </x:si>
   <x:si>
     <x:t>This is a loud line!</x:t>
@@ -268,16 +274,17 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:G20" totalsRowShown="0">
-  <x:autoFilter ref="A1:G20"/>
-  <x:tableColumns count="7">
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H20" totalsRowShown="0">
+  <x:autoFilter ref="A1:H20"/>
+  <x:tableColumns count="8">
     <x:tableColumn id="1" name="ID"/>
     <x:tableColumn id="2" name="Character"/>
     <x:tableColumn id="3" name="Qualifier"/>
-    <x:tableColumn id="4" name="Line"/>
-    <x:tableColumn id="5" name="Direction"/>
-    <x:tableColumn id="6" name="Comments"/>
-    <x:tableColumn id="7" name="Tags"/>
+    <x:tableColumn id="4" name="Actor"/>
+    <x:tableColumn id="5" name="Line"/>
+    <x:tableColumn id="6" name="Direction"/>
+    <x:tableColumn id="7" name="Comments"/>
+    <x:tableColumn id="8" name="Tags"/>
   </x:tableColumns>
   <x:tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </x:table>
@@ -571,7 +578,7 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:G20"/>
+  <x:dimension ref="A1:H20"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
@@ -580,13 +587,14 @@
     <x:col min="1" max="1" width="26.585625" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="11.210625" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="9.835625" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="27.960625" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="10.335625" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="36.835625" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="6.960625" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="7.460625" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="27.960625" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="10.335625" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="36.835625" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="6.960625" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:7">
+    <x:row r="1" spans="1:8">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -608,442 +616,502 @@
       <x:c r="G1" s="1" t="s">
         <x:v>6</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:7">
+      <x:c r="H1" s="1" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:8">
       <x:c r="A2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="D2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E2" s="0" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="G2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H2" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:8">
+      <x:c r="A3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B3" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="F2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G2" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:7">
-      <x:c r="A3" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="B3" s="0" t="s">
-        <x:v>8</x:v>
-      </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
-        <x:v>13</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E3" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="F3" s="0" t="s">
-        <x:v>14</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G3" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:7">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:8">
       <x:c r="A4" s="0" t="s">
-        <x:v>15</x:v>
+        <x:v>16</x:v>
       </x:c>
       <x:c r="B4" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C4" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:8">
+      <x:c r="A5" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-      <x:c r="F4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-      <x:c r="G4" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:7">
-      <x:c r="A5" s="0" t="s">
-        <x:v>19</x:v>
-      </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
       <x:c r="C5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>22</x:v>
       </x:c>
       <x:c r="F5" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G5" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="6" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H5" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:8">
       <x:c r="A6" s="0" t="s">
-        <x:v>21</x:v>
+        <x:v>23</x:v>
       </x:c>
       <x:c r="B6" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D6" s="0" t="s">
-        <x:v>22</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>24</x:v>
       </x:c>
       <x:c r="F6" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G6" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="7" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:8">
       <x:c r="A7" s="0" t="s">
-        <x:v>23</x:v>
+        <x:v>25</x:v>
       </x:c>
       <x:c r="B7" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D7" s="0" t="s">
-        <x:v>24</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>26</x:v>
       </x:c>
       <x:c r="F7" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G7" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="8" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:8">
       <x:c r="A8" s="0" t="s">
-        <x:v>25</x:v>
+        <x:v>27</x:v>
       </x:c>
       <x:c r="B8" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D8" s="0" t="s">
-        <x:v>26</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>28</x:v>
       </x:c>
       <x:c r="F8" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G8" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="9" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:8">
       <x:c r="A9" s="0" t="s">
-        <x:v>27</x:v>
+        <x:v>29</x:v>
       </x:c>
       <x:c r="B9" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D9" s="0" t="s">
-        <x:v>28</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>30</x:v>
       </x:c>
       <x:c r="F9" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G9" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="10" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:8">
       <x:c r="A10" s="0" t="s">
-        <x:v>29</x:v>
+        <x:v>31</x:v>
       </x:c>
       <x:c r="B10" s="0" t="s">
-        <x:v>30</x:v>
+        <x:v>32</x:v>
       </x:c>
       <x:c r="C10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D10" s="0" t="s">
-        <x:v>31</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>33</x:v>
       </x:c>
       <x:c r="F10" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G10" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="11" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="11" spans="1:8">
       <x:c r="A11" s="0" t="s">
-        <x:v>32</x:v>
+        <x:v>34</x:v>
       </x:c>
       <x:c r="B11" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C11" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D11" s="0" t="s">
-        <x:v>33</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E11" s="0" t="s">
-        <x:v>34</x:v>
+        <x:v>35</x:v>
       </x:c>
       <x:c r="F11" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>36</x:v>
       </x:c>
       <x:c r="G11" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="12" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H11" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="12" spans="1:8">
       <x:c r="A12" s="0" t="s">
-        <x:v>35</x:v>
+        <x:v>37</x:v>
       </x:c>
       <x:c r="B12" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C12" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D12" s="0" t="s">
-        <x:v>36</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E12" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>38</x:v>
       </x:c>
       <x:c r="F12" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G12" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="13" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H12" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="13" spans="1:8">
       <x:c r="A13" s="0" t="s">
-        <x:v>37</x:v>
+        <x:v>39</x:v>
       </x:c>
       <x:c r="B13" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C13" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D13" s="0" t="s">
-        <x:v>38</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E13" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>40</x:v>
       </x:c>
       <x:c r="F13" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G13" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="14" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H13" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="14" spans="1:8">
       <x:c r="A14" s="0" t="s">
-        <x:v>39</x:v>
+        <x:v>41</x:v>
       </x:c>
       <x:c r="B14" s="0" t="s">
-        <x:v>40</x:v>
+        <x:v>42</x:v>
       </x:c>
       <x:c r="C14" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D14" s="0" t="s">
-        <x:v>41</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E14" s="0" t="s">
-        <x:v>42</x:v>
+        <x:v>43</x:v>
       </x:c>
       <x:c r="F14" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>44</x:v>
       </x:c>
       <x:c r="G14" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="15" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H14" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="15" spans="1:8">
       <x:c r="A15" s="0" t="s">
-        <x:v>43</x:v>
+        <x:v>45</x:v>
       </x:c>
       <x:c r="B15" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C15" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D15" s="0" t="s">
-        <x:v>44</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E15" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>46</x:v>
       </x:c>
       <x:c r="F15" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G15" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="16" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H15" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="16" spans="1:8">
       <x:c r="A16" s="0" t="s">
-        <x:v>45</x:v>
+        <x:v>47</x:v>
       </x:c>
       <x:c r="B16" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C16" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D16" s="0" t="s">
-        <x:v>46</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E16" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>48</x:v>
       </x:c>
       <x:c r="F16" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G16" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="17" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H16" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="17" spans="1:8">
       <x:c r="A17" s="0" t="s">
-        <x:v>47</x:v>
+        <x:v>49</x:v>
       </x:c>
       <x:c r="B17" s="0" t="s">
-        <x:v>16</x:v>
+        <x:v>17</x:v>
       </x:c>
       <x:c r="C17" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D17" s="0" t="s">
-        <x:v>48</x:v>
+        <x:v>18</x:v>
       </x:c>
       <x:c r="E17" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>50</x:v>
       </x:c>
       <x:c r="F17" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G17" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="18" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H17" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="18" spans="1:8">
       <x:c r="A18" s="0" t="s">
-        <x:v>49</x:v>
+        <x:v>51</x:v>
       </x:c>
       <x:c r="B18" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C18" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D18" s="0" t="s">
-        <x:v>51</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E18" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>53</x:v>
       </x:c>
       <x:c r="F18" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="G18" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="19" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H18" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="19" spans="1:8">
       <x:c r="A19" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="B19" s="0" t="s">
         <x:v>52</x:v>
       </x:c>
-      <x:c r="B19" s="0" t="s">
-        <x:v>50</x:v>
-      </x:c>
       <x:c r="C19" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D19" s="0" t="s">
-        <x:v>53</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="E19" s="0" t="s">
-        <x:v>54</x:v>
+        <x:v>55</x:v>
       </x:c>
       <x:c r="F19" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>56</x:v>
       </x:c>
       <x:c r="G19" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="20" spans="1:7">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H19" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="20" spans="1:8">
       <x:c r="A20" s="0" t="s">
-        <x:v>55</x:v>
+        <x:v>57</x:v>
       </x:c>
       <x:c r="B20" s="0" t="s">
-        <x:v>50</x:v>
+        <x:v>52</x:v>
       </x:c>
       <x:c r="C20" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
       </x:c>
       <x:c r="D20" s="0" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E20" s="0" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="F20" s="0" t="s">
         <x:v>56</x:v>
       </x:c>
-      <x:c r="E20" s="0" t="s">
-        <x:v>54</x:v>
-      </x:c>
-      <x:c r="F20" s="0" t="s">
-        <x:v>9</x:v>
-      </x:c>
       <x:c r="G20" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="H20" s="0" t="s">
+        <x:v>10</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>